<commit_message>
Updated to new APIX YAML format with multiple APIs support
- Added new fields: snowData, gateway, consumers, consumingCountryGroups
- Updated CSV/Excel with HSBC GitHub Enterprise repo data
- Modified YAML generation to match new APIX format
- Removed old metadata structure (apiVersion, kind)
- Added support for apiContractUrl, documentationUrl, apiHostingCountry
</commit_message>
<xml_diff>
--- a/sample_api_data.xlsx
+++ b/sample_api_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,32 +456,67 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>snow_application_service_id</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>platform</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>lifecycle_status</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>classification</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>owner_team</t>
+          <t>api_contract_url</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>contact_email</t>
+          <t>documentation_url</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>api_hosting_country</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>gateway_type</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>gateway_proxy_url</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>gateway_config_url</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>consumer_application_service_ids</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>consuming_country_code</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>consuming_group_member_code</t>
         </is>
       </c>
     </row>
@@ -493,47 +528,82 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>jenkins-mcp-api</t>
+          <t>cto-mmf-hk-hase-pa-customer-accounts</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>v1.0.0</t>
+          <t>1.0.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>APP001234</t>
+          <t>BA0001754</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>gcp</t>
+          <t>AS0003321</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>GCP_OTHER</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>internal</t>
+          <t>ACTIVE</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Jenkins MCP API for CI/CD automation</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>DevOps Team</t>
+          <t>https://example.com/api/contract.yaml</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>devops-team@hsbc.com</t>
+          <t>https://confluence.example.com/api-docs</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>KONG</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>https://proxy.example.com</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>https://config.example.com</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>AS0003321</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>HASE</t>
         </is>
       </c>
     </row>
@@ -550,42 +620,77 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>v2.0.0</t>
+          <t>2.0.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>APP001234</t>
+          <t>BA0001754</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>gcp</t>
+          <t>AS0003322</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>GCP_OTHER</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>internal</t>
+          <t>ACTIVE</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Jenkins Pipeline Management API</t>
+          <t>INTERNAL</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>DevOps Team</t>
+          <t>https://example.com/api/pipeline-contract.yaml</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>devops-team@hsbc.com</t>
+          <t>https://confluence.example.com/pipeline-docs</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>KONG</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>https://proxy.example.com</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>https://config.example.com</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>AS0003322</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>GB</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>HASE</t>
         </is>
       </c>
     </row>
@@ -640,6 +745,13 @@
           <t>payment-team@example.com</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -692,6 +804,13 @@
           <t>payment-team@example.com</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -744,6 +863,13 @@
           <t>identity@example.com</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
+      <c r="Q6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -796,6 +922,13 @@
           <t>supply@example.com</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -848,6 +981,13 @@
           <t>platform@example.com</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -900,6 +1040,13 @@
           <t>legacy@example.com</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -952,6 +1099,13 @@
           <t>analytics@example.com</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1004,6 +1158,13 @@
           <t>search@example.com</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1056,6 +1217,13 @@
           <t>finance@example.com</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>